<commit_message>
Got the files to load properly when they are in the data folder.
</commit_message>
<xml_diff>
--- a/floorMedium.xlsx
+++ b/floorMedium.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Fall '15\Software Engineering\Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kito\Documents\Fall '15\Software Engineering (CSCI306)\workspace\Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="50" windowWidth="23000" windowHeight="10040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="5">
   <si>
     <t>A</t>
   </si>
@@ -448,16 +448,16 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="25" width="3.7109375" customWidth="1"/>
-    <col min="26" max="26" width="5.28515625" customWidth="1"/>
+    <col min="1" max="25" width="3.7265625" customWidth="1"/>
+    <col min="26" max="26" width="5.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -534,7 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -611,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -688,7 +688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -765,7 +765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -842,7 +842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -919,7 +919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -996,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
@@ -1981,7 +1981,9 @@
       <c r="T20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="U20" s="4"/>
+      <c r="U20" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="V20" s="5" t="s">
         <v>4</v>
       </c>
@@ -1995,7 +1997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>4</v>
       </c>
@@ -2072,7 +2074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
@@ -2226,7 +2228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -2303,7 +2305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
@@ -2380,14 +2382,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2409,7 +2411,7 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>

</xml_diff>